<commit_message>
arreglao lo de import cursos (importar estudiantes estaba melo hpta nichestian)
</commit_message>
<xml_diff>
--- a/api/LibroCurso.xlsx
+++ b/api/LibroCurso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19305" windowHeight="6630"/>
+    <workbookView windowWidth="26250" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1282,7 +1282,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Algunas validaciones faltantes en evaluacion e importar
</commit_message>
<xml_diff>
--- a/api/LibroCurso.xlsx
+++ b/api/LibroCurso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26250" windowHeight="10800"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -54,10 +54,10 @@
     <t>Periodo</t>
   </si>
   <si>
-    <t>I123A</t>
-  </si>
-  <si>
-    <t>Impacto Ambiental</t>
+    <t>C123O</t>
+  </si>
+  <si>
+    <t>Seminario de comunicacion oral y escrita</t>
   </si>
   <si>
     <t>2024-1</t>
@@ -1282,14 +1282,14 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="17.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="17.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="20.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="40.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="21.4285714285714" customWidth="1"/>
     <col min="5" max="5" width="18.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="27.2857142857143" customWidth="1"/>

</xml_diff>

<commit_message>
Fix importar cursos, estudiantes, mensajes y tablas rubricas
</commit_message>
<xml_diff>
--- a/api/LibroCurso.xlsx
+++ b/api/LibroCurso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16275" windowHeight="11580"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -54,22 +54,22 @@
     <t>Periodo</t>
   </si>
   <si>
-    <t>C123O</t>
-  </si>
-  <si>
-    <t>Seminario de comunicacion oral y escrita</t>
+    <t>C321C</t>
+  </si>
+  <si>
+    <t>Ciencias de la computación 2</t>
   </si>
   <si>
     <t>2024-1</t>
   </si>
   <si>
-    <t>Sebastian</t>
-  </si>
-  <si>
-    <t>Hernandez</t>
-  </si>
-  <si>
-    <t>kevin@gmail.com</t>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Bolaños</t>
+  </si>
+  <si>
+    <t>kevinorozco@gmail.com</t>
   </si>
   <si>
     <t>Andres</t>
@@ -1329,8 +1329,8 @@
   <sheetPr/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1380,7 +1380,7 @@
     <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
-        <v>1006010600</v>
+        <v>1061701419</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
@@ -1436,7 +1436,7 @@
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="1"/>
@@ -1552,7 +1552,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="kevin@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId1" display="kevinorozco@gmail.com" tooltip="mailto:kevinorozco@gmail.com"/>
     <hyperlink ref="E4" r:id="rId2" display="andres@gmail.com"/>
     <hyperlink ref="E5" r:id="rId3" display="laura@gmail.com" tooltip="mailto:laura@gmail.com"/>
     <hyperlink ref="E6" r:id="rId4" display="oscar@gmail.com" tooltip="mailto:oscar@gmail.com"/>
@@ -1562,7 +1562,7 @@
     <hyperlink ref="E10" r:id="rId8" display="valentina@gmail.com"/>
     <hyperlink ref="E11" r:id="rId9" display="danis@gmail.com"/>
     <hyperlink ref="E12" r:id="rId10" display="salome@gmail.com"/>
-    <hyperlink ref="E13" r:id="rId11" display="mane@gmail.com"/>
+    <hyperlink ref="E13" r:id="rId11" display="mane@gmail.com" tooltip="mailto:mane@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>